<commit_message>
Students Data for All Engineer Cycle Class
</commit_message>
<xml_diff>
--- a/resources/GINF2/students.xlsx
+++ b/resources/GINF2/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E45107-1E66-4BE6-B287-579816369633}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D030FF-C97E-4031-B417-EA3E83625E33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
   </bookViews>
@@ -1098,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF76A2F-C15E-4FF5-B172-1616349AC431}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout de tous les données et mise à jour des CNE
</commit_message>
<xml_diff>
--- a/resources/GINF2/students.xlsx
+++ b/resources/GINF2/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D030FF-C97E-4031-B417-EA3E83625E33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF134DD-522E-4C90-A587-AE93EBA78F3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="8325" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1098,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF76A2F-C15E-4FF5-B172-1616349AC431}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>332</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>335</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>336</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>338</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>339</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>340</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
         <v>82</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>342</v>
       </c>
       <c r="B14" t="s">
         <v>74</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>344</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>346</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>347</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>348</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>350</v>
       </c>
       <c r="B22" t="s">
         <v>83</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>351</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>352</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>353</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>354</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>355</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>356</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>357</v>
       </c>
       <c r="B29" t="s">
         <v>77</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>358</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>359</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>360</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>361</v>
       </c>
       <c r="B33" t="s">
         <v>54</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>362</v>
       </c>
       <c r="B34" t="s">
         <v>31</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>363</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>364</v>
       </c>
       <c r="B36" t="s">
         <v>46</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>365</v>
       </c>
       <c r="B37" t="s">
         <v>80</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>366</v>
       </c>
       <c r="B38" t="s">
         <v>52</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>367</v>
       </c>
       <c r="B39" t="s">
         <v>59</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>368</v>
       </c>
       <c r="B40" t="s">
         <v>68</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>369</v>
       </c>
       <c r="B41" t="s">
         <v>70</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>370</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>371</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>372</v>
       </c>
       <c r="B44" t="s">
         <v>86</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>373</v>
       </c>
       <c r="B45" t="s">
         <v>37</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="B46" t="s">
         <v>55</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>375</v>
       </c>
       <c r="B47" t="s">
         <v>39</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>376</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>377</v>
       </c>
       <c r="B49" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
mise en place sidebar
</commit_message>
<xml_diff>
--- a/resources/GINF2/students.xlsx
+++ b/resources/GINF2/students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF134DD-522E-4C90-A587-AE93EBA78F3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E63801-0755-4CE7-BDBB-6E0E521D8E12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="8325" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1098,18 +1098,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF76A2F-C15E-4FF5-B172-1616349AC431}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" customWidth="1"/>
+    <col min="6" max="6" width="53.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>330</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>331</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>332</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>333</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>334</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>335</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>336</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>337</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>338</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>339</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>340</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>341</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>342</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>343</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>344</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>345</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>346</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>347</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>348</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>349</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>350</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>351</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>352</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>353</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>354</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>355</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>356</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>357</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>358</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>359</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>360</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>361</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>362</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>363</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>364</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>365</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>366</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>367</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>368</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>369</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>370</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>371</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>372</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>373</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>374</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>375</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>376</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>377</v>
       </c>

</xml_diff>